<commit_message>
fixed rule_evaluator for double blank checks
</commit_message>
<xml_diff>
--- a/qa_summary_template.xlsx
+++ b/qa_summary_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luria\PycharmProjects\QAStudiov3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C75A92-8CFF-4353-9FC3-0D63D3E543B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB79BFB-7BD7-42F3-AE0B-ACFE32DDDFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8B1E45A7-8AFB-4663-93E0-BF9D2E7351DE}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t xml:space="preserve">IAG Overall Results and Rating </t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Total Score</t>
-  </si>
-  <si>
-    <t>Continues like columns D&amp; E with columns for each test basically.</t>
   </si>
   <si>
     <t>Score</t>
@@ -130,10 +127,6 @@
 Audit Leader &lt;&gt; Submitter</t>
   </si>
   <si>
-    <t>Rule 2 Title / Name e.g.
-Audit Leader &lt;&gt; Approver</t>
-  </si>
-  <si>
     <t>Weighted Score</t>
   </si>
   <si>
@@ -155,9 +148,6 @@
     <t>Area</t>
   </si>
   <si>
-    <t>Analytics</t>
-  </si>
-  <si>
     <t>IAG-Wide Analytic</t>
   </si>
   <si>
@@ -170,36 +160,15 @@
     <t>Rationale if out of scope within this review</t>
   </si>
   <si>
-    <t>Not Applicable</t>
-  </si>
-  <si>
     <t>Budget Per Sample (Where samples are tested)</t>
   </si>
   <si>
     <t>Total Budget</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>Analytic ID / Sub-Area</t>
   </si>
   <si>
-    <t>QA-ID-1</t>
-  </si>
-  <si>
-    <t>QA-ID-2</t>
-  </si>
-  <si>
-    <t>QA-ID-3</t>
-  </si>
-  <si>
-    <t>QA-ID-4</t>
-  </si>
-  <si>
-    <t>Continues like column D with columns for each test basically.</t>
-  </si>
-  <si>
     <t>Etc.</t>
   </si>
   <si>
@@ -237,42 +206,6 @@
   </si>
   <si>
     <t>{{IAG_TOTAL_COUNT}}</t>
-  </si>
-  <si>
-    <t>{{AUDIT_LEADER_1_NAME}}</t>
-  </si>
-  <si>
-    <t>{{AUDIT_LEADER_1_TEST1_OVERALL RESULT}}</t>
-  </si>
-  <si>
-    <t>{{AUDIT_LEADER_1_TEST2_OVERALL RESULT}}</t>
-  </si>
-  <si>
-    <t>{{AUDIT_LEADER_2_NAME}}</t>
-  </si>
-  <si>
-    <t>{{AUDIT_LEADER_2_TEST1_OVERALL RESULT}}</t>
-  </si>
-  <si>
-    <t>{{AUDIT_LEADER_2_TEST2_OVERALL RESULT}}</t>
-  </si>
-  <si>
-    <t>{{AUDIT_LEADER_3_NAME}}</t>
-  </si>
-  <si>
-    <t>{{AUDIT_LEADER_3_TEST1_OVERALL RESULT}}</t>
-  </si>
-  <si>
-    <t>{{AUDIT_LEADER_3_TEST2_OVERALL RESULT}}</t>
-  </si>
-  <si>
-    <t>{{AUDIT_LEADER_4_NAME}}</t>
-  </si>
-  <si>
-    <t>{{AUDIT_LEADER_4_TEST1_OVERALL RESULT}}</t>
-  </si>
-  <si>
-    <t>{{AUDIT_LEADER_4_TEST2_OVERALL RESULT}}</t>
   </si>
 </sst>
 </file>
@@ -864,9 +797,6 @@
           <cell r="B3" t="str">
             <v>GC</v>
           </cell>
-          <cell r="C3">
-            <v>5</v>
-          </cell>
           <cell r="D3">
             <v>0.8</v>
           </cell>
@@ -875,9 +805,6 @@
           <cell r="B4" t="str">
             <v>PC</v>
           </cell>
-          <cell r="C4">
-            <v>3</v>
-          </cell>
           <cell r="D4">
             <v>0.5</v>
           </cell>
@@ -885,9 +812,6 @@
         <row r="5">
           <cell r="B5" t="str">
             <v>DNC</v>
-          </cell>
-          <cell r="C5">
-            <v>1</v>
           </cell>
         </row>
         <row r="6">
@@ -1223,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC1A94B5-46AB-4193-A6C0-F90FE046489E}">
   <dimension ref="B2:N34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1245,7 +1169,7 @@
   <sheetData>
     <row r="2" spans="2:12" ht="26.25">
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="27" customHeight="1">
@@ -1279,10 +1203,10 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>7</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>8</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="13"/>
@@ -1290,80 +1214,80 @@
     </row>
     <row r="6" spans="2:12">
       <c r="B6" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="16" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J6" s="17"/>
       <c r="L6" s="18"/>
     </row>
     <row r="7" spans="2:12">
       <c r="B7" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="16" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
       <c r="H7" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J7" s="17"/>
       <c r="L7" s="18"/>
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="16" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J8" s="17"/>
       <c r="L8" s="18"/>
     </row>
     <row r="9" spans="2:12">
       <c r="B9" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="16" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J9" s="19"/>
       <c r="K9" s="20"/>
@@ -1371,7 +1295,7 @@
     </row>
     <row r="10" spans="2:12">
       <c r="B10" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="16">
@@ -1384,93 +1308,73 @@
       <c r="H10" s="22"/>
       <c r="I10" s="16"/>
       <c r="J10" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L10" s="22"/>
     </row>
     <row r="11" spans="2:12">
       <c r="B11" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="24" t="str">
         <f>IF(D10="N/A",[1]Configuration!C6, IF(D10&gt;3.9, "GC", IF(D10&lt;2.5, "DNC", "PC")))</f>
         <v>DNC</v>
       </c>
-      <c r="E11" s="24"/>
+      <c r="E11" s="16"/>
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
     </row>
     <row r="13" spans="2:12" ht="18">
       <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="35" t="s">
         <v>17</v>
-      </c>
-      <c r="H13" s="35" t="s">
-        <v>18</v>
       </c>
       <c r="I13" s="35"/>
     </row>
     <row r="14" spans="2:12" ht="31.5" customHeight="1">
       <c r="B14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="4" t="s">
+      <c r="J14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="K14" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" s="15" t="s">
-        <v>58</v>
-      </c>
+      <c r="B15" s="15"/>
       <c r="C15" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="26">
-        <f>(COUNTIFS(D$31:D$35,[1]Configuration!$B$3,$B$31:$B$35,$B15)*[1]Configuration!$C$3) + (COUNTIFS(D$31:D$35,[1]Configuration!$B$4,$B$31:$B$35,$B15)*[1]Configuration!$C$4) + (COUNTIFS(D$31:D$35,[1]Configuration!$B$5,$B$31:$B$35,$B15)*[1]Configuration!$C$5) + (COUNTIFS(D$31:D$35,[1]Configuration!$B$6,$B$31:$B$35,$B15)*[1]Configuration!$C$6)</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="26">
-        <f>(COUNTIFS(E$31:E$35,[1]Configuration!$B$3,$B$31:$B$35,$B15)*[1]Configuration!$C$3) + (COUNTIFS(E$31:E$35,[1]Configuration!$B$4,$B$31:$B$35,$B15)*[1]Configuration!$C$4) + (COUNTIFS(E$31:E$35,[1]Configuration!$B$5,$B$31:$B$35,$B15)*[1]Configuration!$C$5) + (COUNTIFS(E$31:E$35,[1]Configuration!$B$6,$B$31:$B$35,$B15)*[1]Configuration!$C$6)</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="27">
-        <f>(COUNTIFS(F$31:F$35,[1]Configuration!$B$3,$B$31:$B$35,$B15)*[1]Configuration!$C$3) + (COUNTIFS(F$31:F$35,[1]Configuration!$B$4,$B$31:$B$35,$B15)*[1]Configuration!$C$4) + (COUNTIFS(F$31:F$35,[1]Configuration!$B$5,$B$31:$B$35,$B15)*[1]Configuration!$C$5) + (COUNTIFS(F$31:F$35,[1]Configuration!$B$6,$B$31:$B$35,$B15)*[1]Configuration!$C$6)</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="27">
-        <f>(COUNTIFS(G$31:G$35,[1]Configuration!$B$3,$B$31:$B$35,$B15)*[1]Configuration!$C$3) + (COUNTIFS(G$31:G$35,[1]Configuration!$B$4,$B$31:$B$35,$B15)*[1]Configuration!$C$4) + (COUNTIFS(G$31:G$35,[1]Configuration!$B$5,$B$31:$B$35,$B15)*[1]Configuration!$C$5) + (COUNTIFS(G$31:G$35,[1]Configuration!$B$6,$B$31:$B$35,$B15)*[1]Configuration!$C$6)</f>
-        <v>0</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
       <c r="H15" s="16" t="str">
         <f>IF(SUM(D15:G15)=0, "N/A", SUM(D15:G15)/SUMIF(D15:G15,"&lt;&gt;0",D$25:G$25))</f>
         <v>N/A</v>
@@ -1485,36 +1389,22 @@
         <v>N/A</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L15" s="23"/>
     </row>
     <row r="16" spans="2:12">
-      <c r="B16" s="15" t="s">
-        <v>61</v>
-      </c>
+      <c r="B16" s="15"/>
       <c r="C16" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="26">
-        <f>(COUNTIFS(D$31:D$35,[1]Configuration!$B$3,$B$31:$B$35,$B16)*[1]Configuration!$C$3) + (COUNTIFS(D$31:D$35,[1]Configuration!$B$4,$B$31:$B$35,$B16)*[1]Configuration!$C$4) + (COUNTIFS(D$31:D$35,[1]Configuration!$B$5,$B$31:$B$35,$B16)*[1]Configuration!$C$5) + (COUNTIFS(D$31:D$35,[1]Configuration!$B$6,$B$31:$B$35,$B16)*[1]Configuration!$C$6)</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="26">
-        <f>(COUNTIFS(E$31:E$35,[1]Configuration!$B$3,$B$31:$B$35,$B16)*[1]Configuration!$C$3) + (COUNTIFS(E$31:E$35,[1]Configuration!$B$4,$B$31:$B$35,$B16)*[1]Configuration!$C$4) + (COUNTIFS(E$31:E$35,[1]Configuration!$B$5,$B$31:$B$35,$B16)*[1]Configuration!$C$5) + (COUNTIFS(E$31:E$35,[1]Configuration!$B$6,$B$31:$B$35,$B16)*[1]Configuration!$C$6)</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="27">
-        <f>(COUNTIFS(F$31:F$35,[1]Configuration!$B$3,$B$31:$B$35,$B16)*[1]Configuration!$C$3) + (COUNTIFS(F$31:F$35,[1]Configuration!$B$4,$B$31:$B$35,$B16)*[1]Configuration!$C$4) + (COUNTIFS(F$31:F$35,[1]Configuration!$B$5,$B$31:$B$35,$B16)*[1]Configuration!$C$5) + (COUNTIFS(F$31:F$35,[1]Configuration!$B$6,$B$31:$B$35,$B16)*[1]Configuration!$C$6)</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="27">
-        <f>(COUNTIFS(G$31:G$35,[1]Configuration!$B$3,$B$31:$B$35,$B16)*[1]Configuration!$C$3) + (COUNTIFS(G$31:G$35,[1]Configuration!$B$4,$B$31:$B$35,$B16)*[1]Configuration!$C$4) + (COUNTIFS(G$31:G$35,[1]Configuration!$B$5,$B$31:$B$35,$B16)*[1]Configuration!$C$5) + (COUNTIFS(G$31:G$35,[1]Configuration!$B$6,$B$31:$B$35,$B16)*[1]Configuration!$C$6)</f>
-        <v>0</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
       <c r="H16" s="16" t="str">
         <f>IF(SUM(D16:G16)=0, "N/A", SUM(D16:G16)/SUMIF(D16:G16,"&lt;&gt;0",D$25:G$25))</f>
         <v>N/A</v>
@@ -1529,36 +1419,22 @@
         <v>N/A</v>
       </c>
       <c r="J16" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L16" s="23"/>
     </row>
     <row r="17" spans="2:14">
-      <c r="B17" s="15" t="s">
-        <v>64</v>
-      </c>
+      <c r="B17" s="15"/>
       <c r="C17" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="26">
-        <f>(COUNTIFS(D$31:D$35,[1]Configuration!$B$3,$B$31:$B$35,$B17)*[1]Configuration!$C$3) + (COUNTIFS(D$31:D$35,[1]Configuration!$B$4,$B$31:$B$35,$B17)*[1]Configuration!$C$4) + (COUNTIFS(D$31:D$35,[1]Configuration!$B$5,$B$31:$B$35,$B17)*[1]Configuration!$C$5) + (COUNTIFS(D$31:D$35,[1]Configuration!$B$6,$B$31:$B$35,$B17)*[1]Configuration!$C$6)</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="26">
-        <f>(COUNTIFS(E$31:E$35,[1]Configuration!$B$3,$B$31:$B$35,$B17)*[1]Configuration!$C$3) + (COUNTIFS(E$31:E$35,[1]Configuration!$B$4,$B$31:$B$35,$B17)*[1]Configuration!$C$4) + (COUNTIFS(E$31:E$35,[1]Configuration!$B$5,$B$31:$B$35,$B17)*[1]Configuration!$C$5) + (COUNTIFS(E$31:E$35,[1]Configuration!$B$6,$B$31:$B$35,$B17)*[1]Configuration!$C$6)</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="27">
-        <f>(COUNTIFS(F$31:F$35,[1]Configuration!$B$3,$B$31:$B$35,$B17)*[1]Configuration!$C$3) + (COUNTIFS(F$31:F$35,[1]Configuration!$B$4,$B$31:$B$35,$B17)*[1]Configuration!$C$4) + (COUNTIFS(F$31:F$35,[1]Configuration!$B$5,$B$31:$B$35,$B17)*[1]Configuration!$C$5) + (COUNTIFS(F$31:F$35,[1]Configuration!$B$6,$B$31:$B$35,$B17)*[1]Configuration!$C$6)</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="27">
-        <f>(COUNTIFS(G$31:G$35,[1]Configuration!$B$3,$B$31:$B$35,$B17)*[1]Configuration!$C$3) + (COUNTIFS(G$31:G$35,[1]Configuration!$B$4,$B$31:$B$35,$B17)*[1]Configuration!$C$4) + (COUNTIFS(G$31:G$35,[1]Configuration!$B$5,$B$31:$B$35,$B17)*[1]Configuration!$C$5) + (COUNTIFS(G$31:G$35,[1]Configuration!$B$6,$B$31:$B$35,$B17)*[1]Configuration!$C$6)</f>
-        <v>0</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
       <c r="H17" s="16" t="str">
         <f>IF(SUM(D17:G17)=0, "N/A", SUM(D17:G17)/SUMIF(D17:G17,"&lt;&gt;0",D$25:G$25))</f>
         <v>N/A</v>
@@ -1573,36 +1449,22 @@
         <v>N/A</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L17" s="23"/>
     </row>
     <row r="18" spans="2:14">
-      <c r="B18" s="15" t="s">
-        <v>67</v>
-      </c>
+      <c r="B18" s="15"/>
       <c r="C18" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="26">
-        <f>(COUNTIFS(D$31:D$35,[1]Configuration!$B$3,$B$31:$B$35,$B18)*[1]Configuration!$C$3) + (COUNTIFS(D$31:D$35,[1]Configuration!$B$4,$B$31:$B$35,$B18)*[1]Configuration!$C$4) + (COUNTIFS(D$31:D$35,[1]Configuration!$B$5,$B$31:$B$35,$B18)*[1]Configuration!$C$5) + (COUNTIFS(D$31:D$35,[1]Configuration!$B$6,$B$31:$B$35,$B18)*[1]Configuration!$C$6)</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="26">
-        <f>(COUNTIFS(E$31:E$35,[1]Configuration!$B$3,$B$31:$B$35,$B18)*[1]Configuration!$C$3) + (COUNTIFS(E$31:E$35,[1]Configuration!$B$4,$B$31:$B$35,$B18)*[1]Configuration!$C$4) + (COUNTIFS(E$31:E$35,[1]Configuration!$B$5,$B$31:$B$35,$B18)*[1]Configuration!$C$5) + (COUNTIFS(E$31:E$35,[1]Configuration!$B$6,$B$31:$B$35,$B18)*[1]Configuration!$C$6)</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="27">
-        <f>(COUNTIFS(F$31:F$35,[1]Configuration!$B$3,$B$31:$B$35,$B18)*[1]Configuration!$C$3) + (COUNTIFS(F$31:F$35,[1]Configuration!$B$4,$B$31:$B$35,$B18)*[1]Configuration!$C$4) + (COUNTIFS(F$31:F$35,[1]Configuration!$B$5,$B$31:$B$35,$B18)*[1]Configuration!$C$5) + (COUNTIFS(F$31:F$35,[1]Configuration!$B$6,$B$31:$B$35,$B18)*[1]Configuration!$C$6)</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="27">
-        <f>(COUNTIFS(G$31:G$35,[1]Configuration!$B$3,$B$31:$B$35,$B18)*[1]Configuration!$C$3) + (COUNTIFS(G$31:G$35,[1]Configuration!$B$4,$B$31:$B$35,$B18)*[1]Configuration!$C$4) + (COUNTIFS(G$31:G$35,[1]Configuration!$B$5,$B$31:$B$35,$B18)*[1]Configuration!$C$5) + (COUNTIFS(G$31:G$35,[1]Configuration!$B$6,$B$31:$B$35,$B18)*[1]Configuration!$C$6)</f>
-        <v>0</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
       <c r="H18" s="16" t="str">
         <f>IF(SUM(D18:G18)=0, "N/A", SUM(D18:G18)/SUMIF(D18:G18,"&lt;&gt;0",D$25:G$25))</f>
         <v>N/A</v>
@@ -1617,41 +1479,33 @@
         <v>N/A</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L18" s="23"/>
     </row>
     <row r="21" spans="2:14" ht="18">
       <c r="B21" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="2:14" ht="18">
       <c r="B22" s="3"/>
       <c r="C22" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" s="29" t="s">
-        <v>30</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
       <c r="H22" s="29"/>
     </row>
     <row r="23" spans="2:14" ht="18">
       <c r="B23" s="3"/>
       <c r="C23" s="28" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D23" s="29"/>
       <c r="E23" s="29"/>
@@ -1662,114 +1516,63 @@
     <row r="24" spans="2:14" ht="18">
       <c r="B24" s="3"/>
       <c r="C24" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="30">
-        <v>0.02</v>
-      </c>
-      <c r="E24" s="30">
-        <v>0.02</v>
-      </c>
-      <c r="F24" s="30">
-        <v>0</v>
-      </c>
-      <c r="G24" s="30">
-        <v>0.01</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
       <c r="H24" s="29"/>
     </row>
     <row r="25" spans="2:14" ht="18">
       <c r="B25" s="3"/>
       <c r="C25" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="29">
-        <v>3</v>
-      </c>
-      <c r="E25" s="29">
-        <v>3</v>
-      </c>
-      <c r="F25" s="29">
-        <v>1</v>
-      </c>
-      <c r="G25" s="29">
-        <v>2</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
       <c r="H25" s="29"/>
     </row>
     <row r="26" spans="2:14">
       <c r="C26" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F26" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26" s="29" t="s">
-        <v>35</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
       <c r="H26" s="29"/>
     </row>
     <row r="27" spans="2:14">
       <c r="C27" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="G27" s="29" t="s">
-        <v>35</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
       <c r="H27" s="29"/>
     </row>
     <row r="28" spans="2:14">
       <c r="C28" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F28" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="G28" s="29" t="s">
-        <v>35</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
       <c r="H28" s="29"/>
-      <c r="I28" s="2" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="29" spans="2:14">
       <c r="C29" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="F29" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="G29" s="29" t="s">
-        <v>43</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
       <c r="H29" s="29"/>
       <c r="I29" s="29"/>
       <c r="J29" s="29"/>
@@ -1780,228 +1583,98 @@
     </row>
     <row r="30" spans="2:14" ht="38.25">
       <c r="B30" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>44</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
       <c r="H30" s="4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="L30" s="32" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="M30" s="32" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="N30" s="32" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="2:14">
-      <c r="B31" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="33">
-        <v>0</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>60</v>
-      </c>
+      <c r="B31" s="15"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
-      <c r="I31" s="22">
-        <f>COUNTIF($D31:$G31,"GC")</f>
-        <v>0</v>
-      </c>
-      <c r="J31" s="22">
-        <f>COUNTIF($D31:$G31,"PC")</f>
-        <v>0</v>
-      </c>
-      <c r="K31" s="22">
-        <f>COUNTIF($D31:$G31,"DNC")</f>
-        <v>0</v>
-      </c>
-      <c r="L31" s="22">
-        <f>SUM(I31:K31)</f>
-        <v>0</v>
-      </c>
-      <c r="M31" s="34" t="str">
-        <f>IF(OR(L31=0, [1]Configuration!$C$3=0), "N/A", ((I31*[1]Configuration!$C$3) + (J31*[1]Configuration!$C$4) + (K31*[1]Configuration!$C$5)) / (L31*[1]Configuration!$C$3))</f>
-        <v>N/A</v>
-      </c>
-      <c r="N31" s="16" t="str" cm="1">
-        <f t="array" ref="N31">_xlfn.IFS(
-  M31 = [1]Configuration!$B$6, [1]Configuration!$B$6,
-  M31 &gt;= [1]Configuration!$D$3, [1]Configuration!$B$3,
-  M31 &lt; [1]Configuration!$D$4, [1]Configuration!$B$5,
-  TRUE, [1]Configuration!$B$4
-)</f>
-        <v>N/A</v>
-      </c>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="16"/>
     </row>
     <row r="32" spans="2:14">
-      <c r="B32" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="15">
-        <v>0</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>63</v>
-      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
       <c r="F32" s="16"/>
       <c r="G32" s="16"/>
       <c r="H32" s="16"/>
-      <c r="I32" s="22">
-        <f>COUNTIF($D32:$G32,"GC")</f>
-        <v>0</v>
-      </c>
-      <c r="J32" s="22">
-        <f>COUNTIF($D32:$G32,"PC")</f>
-        <v>0</v>
-      </c>
-      <c r="K32" s="22">
-        <f>COUNTIF($D32:$G32,"DNC")</f>
-        <v>0</v>
-      </c>
-      <c r="L32" s="22">
-        <f>SUM(I32:K32)</f>
-        <v>0</v>
-      </c>
-      <c r="M32" s="34" t="str">
-        <f>IF(OR(L32=0, [1]Configuration!$C$3=0), "N/A", ((I32*[1]Configuration!$C$3) + (J32*[1]Configuration!$C$4) + (K32*[1]Configuration!$C$5)) / (L32*[1]Configuration!$C$3))</f>
-        <v>N/A</v>
-      </c>
-      <c r="N32" s="16" t="str" cm="1">
-        <f t="array" ref="N32">_xlfn.IFS(
-  M32 = [1]Configuration!$B$6, [1]Configuration!$B$6,
-  M32 &gt;= [1]Configuration!$D$3, [1]Configuration!$B$3,
-  M32 &lt; [1]Configuration!$D$4, [1]Configuration!$B$5,
-  TRUE, [1]Configuration!$B$4
-)</f>
-        <v>N/A</v>
-      </c>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="34"/>
+      <c r="N32" s="16"/>
     </row>
     <row r="33" spans="2:14">
-      <c r="B33" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="15">
-        <v>0</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>66</v>
-      </c>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
       <c r="H33" s="16"/>
-      <c r="I33" s="22">
-        <f>COUNTIF($D33:$G33,"GC")</f>
-        <v>0</v>
-      </c>
-      <c r="J33" s="22">
-        <f>COUNTIF($D33:$G33,"PC")</f>
-        <v>0</v>
-      </c>
-      <c r="K33" s="22">
-        <f>COUNTIF($D33:$G33,"DNC")</f>
-        <v>0</v>
-      </c>
-      <c r="L33" s="22">
-        <f>SUM(I33:K33)</f>
-        <v>0</v>
-      </c>
-      <c r="M33" s="34" t="str">
-        <f>IF(OR(L33=0, [1]Configuration!$C$3=0), "N/A", ((I33*[1]Configuration!$C$3) + (J33*[1]Configuration!$C$4) + (K33*[1]Configuration!$C$5)) / (L33*[1]Configuration!$C$3))</f>
-        <v>N/A</v>
-      </c>
-      <c r="N33" s="16" t="str" cm="1">
-        <f t="array" ref="N33">_xlfn.IFS(
-  M33 = [1]Configuration!$B$6, [1]Configuration!$B$6,
-  M33 &gt;= [1]Configuration!$D$3, [1]Configuration!$B$3,
-  M33 &lt; [1]Configuration!$D$4, [1]Configuration!$B$5,
-  TRUE, [1]Configuration!$B$4
-)</f>
-        <v>N/A</v>
-      </c>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="16"/>
     </row>
     <row r="34" spans="2:14">
-      <c r="B34" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="15">
-        <v>0</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>69</v>
-      </c>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
       <c r="H34" s="16"/>
-      <c r="I34" s="22">
-        <f>COUNTIF($D34:$G34,"GC")</f>
-        <v>0</v>
-      </c>
-      <c r="J34" s="22">
-        <f>COUNTIF($D34:$G34,"PC")</f>
-        <v>0</v>
-      </c>
-      <c r="K34" s="22">
-        <f>COUNTIF($D34:$G34,"DNC")</f>
-        <v>0</v>
-      </c>
-      <c r="L34" s="22">
-        <f>SUM(I34:K34)</f>
-        <v>0</v>
-      </c>
-      <c r="M34" s="34" t="str">
-        <f>IF(OR(L34=0, [1]Configuration!$C$3=0), "N/A", ((I34*[1]Configuration!$C$3) + (J34*[1]Configuration!$C$4) + (K34*[1]Configuration!$C$5)) / (L34*[1]Configuration!$C$3))</f>
-        <v>N/A</v>
-      </c>
-      <c r="N34" s="16" t="str" cm="1">
-        <f t="array" ref="N34">_xlfn.IFS(
-  M34 = [1]Configuration!$B$6, [1]Configuration!$B$6,
-  M34 &gt;= [1]Configuration!$D$3, [1]Configuration!$B$3,
-  M34 &lt; [1]Configuration!$D$4, [1]Configuration!$B$5,
-  TRUE, [1]Configuration!$B$4
-)</f>
-        <v>N/A</v>
-      </c>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="34"/>
+      <c r="N34" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>